<commit_message>
add makefile for gcc
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24030" windowHeight="13545"/>
+    <workbookView windowWidth="24030" windowHeight="13545" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85">
   <si>
     <t>FLAGS</t>
   </si>
@@ -111,31 +111,166 @@
     <t>-no-vec -O2 -qopt-matmul</t>
   </si>
   <si>
-    <t>gcc -Ofast</t>
-  </si>
-  <si>
-    <t>norm resid      resid           machep         x[0]-1          x[n-1]-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   1.7    4.00543213e-05   1.19209290e-07  -1.38282776e-05  -7.51018524e-06</t>
-  </si>
-  <si>
-    <t>icc -fast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   1.9    4.57763672e-05   1.19209290e-07  -1.31130219e-05  -1.30534172e-05</t>
-  </si>
-  <si>
-    <t>icc -O1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   1.6    3.80277634e-05   1.19209290e-07  -1.38282776e-05  -7.51018524e-06</t>
-  </si>
-  <si>
-    <t>icc -O2</t>
-  </si>
-  <si>
-    <t>icc -O3</t>
+    <t>-qopt-prefetch -qopt-prefetch-issue-excl-hint</t>
+  </si>
+  <si>
+    <t>-qopt-subscript-in-range</t>
+  </si>
+  <si>
+    <t>-use-intel-optimized-headers</t>
+  </si>
+  <si>
+    <t>-O1 -finline</t>
+  </si>
+  <si>
+    <t>-O1 -falign-functions</t>
+  </si>
+  <si>
+    <t>-O1 -ipo  -xHost   -fno-alias -fargument-noalias -fargument-noalias-global   -qopt-prefetch=1     -fbuiltin     -falign-functions</t>
+  </si>
+  <si>
+    <t>-O2 -ipo     -xHost     -fno-alias -fargument-noalias -fargument-noalias-global   -qopt-prefetch=1     -fbuiltin     -falign-functions</t>
+  </si>
+  <si>
+    <t>GCC Compiler Options</t>
+  </si>
+  <si>
+    <t>-fhosted</t>
+  </si>
+  <si>
+    <t>-fmerge-all-constants</t>
+  </si>
+  <si>
+    <t>-ftree-loop-if-convert</t>
+  </si>
+  <si>
+    <t>-fmodulo-sched</t>
+  </si>
+  <si>
+    <t>-ftree-parallelize-loops=n</t>
+  </si>
+  <si>
+    <t>-fmodulo-sched-allow-regmoves</t>
+  </si>
+  <si>
+    <t>-ftree-loop-vectorize</t>
+  </si>
+  <si>
+    <t>-fgcse-sm</t>
+  </si>
+  <si>
+    <t>-ftree-slp-vectorize</t>
+  </si>
+  <si>
+    <t>-fgcse-after-reload</t>
+  </si>
+  <si>
+    <t>-funsafe-loop-optimizations</t>
+  </si>
+  <si>
+    <t>-fcrossjumping</t>
+  </si>
+  <si>
+    <t>-freschedule-modulo-scheduled-loops</t>
+  </si>
+  <si>
+    <t>-fsemantic-interposition</t>
+  </si>
+  <si>
+    <t>-fipa-pta</t>
+  </si>
+  <si>
+    <t>-ftree-loop-linear</t>
+  </si>
+  <si>
+    <t>-floop-interchange</t>
+  </si>
+  <si>
+    <t>-floop-strip-mine</t>
+  </si>
+  <si>
+    <t>-floop-block</t>
+  </si>
+  <si>
+    <t>-fgraphite-identity</t>
+  </si>
+  <si>
+    <t>-floop-nest-optimize</t>
+  </si>
+  <si>
+    <t>-floop-unroll-and-jam</t>
+  </si>
+  <si>
+    <t>-floop-parallelize-all</t>
+  </si>
+  <si>
+    <t>-ftree-loop-if-convert-stores</t>
+  </si>
+  <si>
+    <t>-ftree-loop-distribution</t>
+  </si>
+  <si>
+    <t>-ftree-loop-im</t>
+  </si>
+  <si>
+    <t>-ftree-loop-ivcanon</t>
+  </si>
+  <si>
+    <t>-fivopts</t>
+  </si>
+  <si>
+    <t>-ftree-coalesce-inlined-vars</t>
+  </si>
+  <si>
+    <t>-ftree-vectorizeu</t>
+  </si>
+  <si>
+    <t>-fvect-cost-model=model</t>
+  </si>
+  <si>
+    <t>-fsimd-cost-model=model</t>
+  </si>
+  <si>
+    <t>-fvariable-expansion-in-unroller</t>
+  </si>
+  <si>
+    <t>-fprefetch-loop-arrays</t>
+  </si>
+  <si>
+    <t>-fwhole-program</t>
+  </si>
+  <si>
+    <t>-flto[=n]</t>
+  </si>
+  <si>
+    <t>-fuse-linker-plugin</t>
+  </si>
+  <si>
+    <t>-fprofile-generate</t>
+  </si>
+  <si>
+    <t>-fprofile-use</t>
+  </si>
+  <si>
+    <t>‘-fno-math-errno’, ‘-funsafe-math-optimizations’,</t>
+  </si>
+  <si>
+    <t>-ffast-math</t>
+  </si>
+  <si>
+    <t>‘-ffinite-math-only’, ‘-fno-rounding-math’, ‘-fno-signaling-nans’ and</t>
+  </si>
+  <si>
+    <t>-freciprocal-math</t>
+  </si>
+  <si>
+    <t>‘-fcx-limited-range</t>
+  </si>
+  <si>
+    <t>-fassociative-math</t>
+  </si>
+  <si>
+    <t>-fno-trapping-math</t>
   </si>
 </sst>
 </file>
@@ -143,12 +278,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -159,21 +294,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -201,30 +321,23 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -239,48 +352,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -302,9 +376,33 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -314,6 +412,36 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -324,192 +452,192 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -609,9 +737,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -621,6 +751,24 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -640,26 +788,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -690,17 +829,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -709,94 +848,94 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -805,58 +944,67 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -891,19 +1039,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -916,6 +1064,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1233,451 +1384,582 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="18.0083333333333" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.2333333333333" style="2" customWidth="1"/>
-    <col min="3" max="5" width="12.2333333333333" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.2333333333333" style="1" customWidth="1"/>
-    <col min="7" max="10" width="12.2333333333333" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="9" style="4"/>
+    <col min="1" max="1" width="18.0083333333333" style="4" customWidth="1"/>
+    <col min="2" max="2" width="12.2333333333333" style="5" customWidth="1"/>
+    <col min="3" max="5" width="12.2333333333333" style="6" customWidth="1"/>
+    <col min="6" max="6" width="12.2333333333333" style="4" customWidth="1"/>
+    <col min="7" max="10" width="12.2333333333333" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="9" style="7"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:7">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="18" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:10">
-      <c r="A2" s="8"/>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="11"/>
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="20"/>
-      <c r="G2" s="2" t="s">
+      <c r="F2" s="23"/>
+      <c r="G2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:10">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="13">
         <v>6.539526</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="14">
         <v>4.529364</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="14">
         <v>2753.79</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="14">
         <v>2747.52</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="6">
         <v>5.8552</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="6">
         <v>2.455303</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="6">
         <v>5646.5</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="6">
         <v>6018.49</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:5">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="5">
         <v>4.615054</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="6">
         <v>4.383118</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="6">
         <v>2661.98</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="6">
         <v>2699.61</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:5">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="13">
         <v>4.649498</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="14">
         <v>5.609066</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="6">
         <v>1933.36</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="6">
         <v>2059.33</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:5">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="5">
         <v>3.65436</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="6">
         <v>4.602692</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="6">
         <v>2508.26</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="6">
         <v>2650.53</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:5">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="13">
         <v>4.866316</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="14">
         <v>4.373621</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="6">
         <v>2710.17</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="6">
         <v>2710.17</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:5">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="5">
         <v>6.556787</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="6">
         <v>4.562157</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="6">
         <v>2738.4</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="6">
         <v>2694.26</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:5">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="5">
         <v>6.573022</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="6">
         <v>4.579344</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="6">
         <v>2662.76</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" customHeight="1" spans="1:5">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="15">
         <v>6.53494</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="6">
         <v>4.580584</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="6">
         <v>2730.55</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="6">
         <v>2725.3</v>
       </c>
     </row>
     <row r="11" customHeight="1" spans="1:5">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="6">
         <v>6.678084</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="14">
         <v>4.172291</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="14">
         <v>3029.93</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="14">
         <v>3042.83</v>
       </c>
     </row>
     <row r="12" customHeight="1" spans="1:5">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="16">
         <v>4.758976</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="14">
         <v>4.335672</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="14">
         <v>2826.06</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="14">
         <v>2801.12</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="1:5">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="5">
         <v>6.441762</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="6">
         <v>4.577482</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="6">
         <v>2783.76</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="6">
         <v>2711.28</v>
       </c>
     </row>
     <row r="14" customHeight="1" spans="1:5">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="5">
         <v>6.529734</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="6">
         <v>4.586468</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="6">
         <v>2515.4</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="6">
         <v>2577.42</v>
       </c>
     </row>
     <row r="15" customHeight="1" spans="1:5">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="5">
         <v>6.620865</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="6">
         <v>4.520092</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="6">
         <v>2743.92</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="6">
         <v>2743.68</v>
       </c>
     </row>
     <row r="16" customHeight="1" spans="1:5">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="13">
         <v>6.98274</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="14">
         <v>4.939034</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="6">
         <v>2529.62</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="17" customHeight="1" spans="1:5">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="13">
         <v>4.748555</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C17" s="14">
         <v>4.012024</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="14">
         <v>3021.9</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="14">
         <v>3054.94</v>
       </c>
     </row>
     <row r="18" customHeight="1" spans="1:5">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="5">
         <v>6.52506</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="6">
         <v>4.576473</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="6">
         <v>2716.65</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="6">
         <v>2728.37</v>
       </c>
     </row>
     <row r="19" customHeight="1" spans="1:5">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="5">
         <v>6.537611</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="6">
         <v>4.593819</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="6">
         <v>2697.3</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="6">
         <v>2703.37</v>
       </c>
     </row>
     <row r="20" customHeight="1" spans="1:5">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="5">
         <v>6.537611</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="6">
         <v>4.593819</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="6">
         <v>2697.3</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="6">
         <v>2703.37</v>
       </c>
     </row>
     <row r="21" customHeight="1" spans="1:5">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="5">
         <v>6.501938</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="6">
         <v>4.501932</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="6">
         <v>2772.09</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="6">
         <v>2724.6</v>
       </c>
     </row>
     <row r="22" customHeight="1" spans="1:5">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="5">
         <v>6.503634</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="6">
         <v>4.504871</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="6">
         <v>2707.95</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="6">
         <v>2728.23</v>
       </c>
     </row>
-    <row r="23" customHeight="1" spans="1:2">
-      <c r="A23" s="1" t="s">
+    <row r="23" customHeight="1" spans="1:5">
+      <c r="A23" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="5">
         <v>6.667541</v>
       </c>
+      <c r="C23" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="24" customHeight="1" spans="1:5">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="5">
         <v>4.539174</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="6">
         <v>4.312164</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="6">
         <v>2729.04</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="6">
         <v>2755.5</v>
       </c>
     </row>
+    <row r="25" customHeight="1" spans="1:5">
+      <c r="A25" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="5">
+        <v>6.542594</v>
+      </c>
+      <c r="C25" s="6">
+        <v>4.543344</v>
+      </c>
+      <c r="D25" s="6">
+        <v>2756.04</v>
+      </c>
+      <c r="E25" s="6">
+        <v>2755.13</v>
+      </c>
+    </row>
+    <row r="26" customHeight="1" spans="1:5">
+      <c r="A26" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="5">
+        <v>6.536299</v>
+      </c>
+      <c r="C26" s="6">
+        <v>4.519663</v>
+      </c>
+      <c r="D26" s="6">
+        <v>2725.62</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" customHeight="1" spans="1:5">
+      <c r="A27" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="5">
+        <v>6.540967</v>
+      </c>
+      <c r="C27" s="6">
+        <v>4.511589</v>
+      </c>
+      <c r="D27" s="6">
+        <v>2756.67</v>
+      </c>
+      <c r="E27" s="6">
+        <v>2746.79</v>
+      </c>
+    </row>
+    <row r="28" customHeight="1" spans="1:4">
+      <c r="A28" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="5">
+        <v>6.573017</v>
+      </c>
+      <c r="C28" s="6">
+        <v>4.576862</v>
+      </c>
+      <c r="D28" s="6">
+        <v>2742.48</v>
+      </c>
+    </row>
+    <row r="29" customHeight="1" spans="1:4">
+      <c r="A29" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="5">
+        <v>6.508806</v>
+      </c>
+      <c r="C29" s="6">
+        <v>4.558767</v>
+      </c>
+      <c r="D29" s="6">
+        <v>2703.39</v>
+      </c>
+    </row>
+    <row r="30" customHeight="1" spans="1:5">
+      <c r="A30" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="24"/>
+    </row>
+    <row r="31" customHeight="1" spans="2:5">
+      <c r="B31" s="5">
+        <v>4.834368</v>
+      </c>
+      <c r="C31" s="6">
+        <v>3.589312</v>
+      </c>
+      <c r="D31" s="6">
+        <v>3419.93</v>
+      </c>
+      <c r="E31" s="6">
+        <v>3402.25</v>
+      </c>
+    </row>
+    <row r="32" customHeight="1" spans="1:1">
+      <c r="A32" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" customHeight="1" spans="2:5">
+      <c r="B33" s="5">
+        <v>3.627814</v>
+      </c>
+      <c r="C33" s="6">
+        <v>4.062117</v>
+      </c>
+      <c r="D33" s="6">
+        <v>2925.52</v>
+      </c>
+      <c r="E33" s="6">
+        <v>2925.52</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="G1:J1"/>
+    <mergeCell ref="A30:E30"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="F1:F2"/>
   </mergeCells>
@@ -1689,90 +1971,250 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:A20"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="12.0583333333333" defaultRowHeight="24" customHeight="1" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="22.275" style="1" customWidth="1"/>
+    <col min="2" max="3" width="12.0583333333333" customWidth="1"/>
+    <col min="4" max="4" width="12.0583333333333" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="12.0583333333333" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
+    <row r="1" customHeight="1" spans="1:6">
+      <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" customHeight="1" spans="1:1">
+      <c r="A2" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
-        <v>37</v>
+    <row r="3" customHeight="1" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" customHeight="1" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" customHeight="1" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" customHeight="1" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" customHeight="1" spans="1:1">
+      <c r="A7" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" customHeight="1" spans="1:1">
+      <c r="A8" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" customHeight="1" spans="1:1">
+      <c r="A9" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" customHeight="1" spans="1:1">
+      <c r="A10" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" customHeight="1" spans="1:1">
+      <c r="A11" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" customHeight="1" spans="1:1">
+      <c r="A12" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" customHeight="1" spans="1:1">
+      <c r="A13" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" customHeight="1" spans="1:1">
+      <c r="A14" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" customHeight="1" spans="1:1">
+      <c r="A15" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" customHeight="1" spans="1:1">
+      <c r="A16" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" customHeight="1" spans="1:1">
+      <c r="A17" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" customHeight="1" spans="1:1">
+      <c r="A18" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" customHeight="1" spans="1:1">
+      <c r="A19" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" customHeight="1" spans="1:1">
+      <c r="A20" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" customHeight="1" spans="1:1">
+      <c r="A21" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" customHeight="1" spans="1:1">
+      <c r="A22" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" customHeight="1" spans="1:1">
+      <c r="A23" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" customHeight="1" spans="1:1">
+      <c r="A24" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" customHeight="1" spans="1:1">
+      <c r="A25" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" customHeight="1" spans="1:1">
+      <c r="A26" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" customHeight="1" spans="1:1">
+      <c r="A27" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" customHeight="1" spans="1:1">
+      <c r="A28" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" customHeight="1" spans="1:1">
+      <c r="A29" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" customHeight="1" spans="1:1">
+      <c r="A30" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" customHeight="1" spans="1:1">
+      <c r="A31" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" customHeight="1" spans="1:1">
+      <c r="A32" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" customHeight="1" spans="1:1">
+      <c r="A33" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" customHeight="1" spans="1:1">
+      <c r="A34" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" customHeight="1" spans="1:1">
+      <c r="A35" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" customHeight="1" spans="1:3">
+      <c r="A36" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" customHeight="1" spans="1:3">
+      <c r="A37" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" customHeight="1" spans="1:3">
+      <c r="A38" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" customHeight="1" spans="1:1">
+      <c r="A39" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" customHeight="1" spans="1:1">
+      <c r="A40" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>

</xml_diff>